<commit_message>
Apoorav & Mama ka code
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -3,19 +3,15 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\seleniumworkspaces\LiveProjects\PageObjectwithFactories\src\test\resources\excel\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17205" windowHeight="5370"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15300" windowHeight="2910"/>
   </bookViews>
   <sheets>
     <sheet name="SignInTest" sheetId="1" r:id="rId1"/>
     <sheet name="FlightSearchTest" sheetId="4" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -408,10 +404,13 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="28.5703125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">

</xml_diff>